<commit_message>
Update data package at: 2025-09-25T17:48:29Z
</commit_message>
<xml_diff>
--- a/data/checks-planejamento.xlsx
+++ b/data/checks-planejamento.xlsx
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 10 está com os valores totais de receita e despesa diferentes nas bases. R$ 86.620.564.073,00 na base orçamento fiscal da receita, e 92.913.813.925,00 na qdd fiscal. A diferença é de R$ -6293249852.</t>
+          <t>A Fonte de Recurso 10 está com os valores totais de receita e despesa diferentes nas bases. R$ 84.363.501.073,00 na base orçamento fiscal da receita, e 90.656.750.925,00 na qdd fiscal. A diferença é de R$ -6293249852.</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>A uo 1451 está com uma diferença de R$ (1.778.147,00) entre o valor de limite no ano 0 (R$ 41.116.142,00) e a soma do valor utilizado no ano (R$ 42.894.289,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 42.894.289,00.</t>
+          <t>A uo 1451 está com uma diferença de R$ (150.714.182,00) entre o valor de limite no ano 0 (R$ 353.708.669,00) e a soma do valor utilizado no ano (R$ 504.422.851,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 504.422.851,00.</t>
         </is>
       </c>
     </row>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>A uo 1451 está com uma diferença de R$ (150.714.182,00) entre o valor de limite no ano 0 (R$ 353.708.669,00) e a soma do valor utilizado no ano (R$ 504.422.851,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 504.422.851,00.</t>
+          <t>A uo 1451 está com uma diferença de R$ (1.778.147,00) entre o valor de limite no ano 0 (R$ 41.116.142,00) e a soma do valor utilizado no ano (R$ 42.894.289,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 42.894.289,00.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data package at: 2026-01-20T13:25:28Z
</commit_message>
<xml_diff>
--- a/data/checks-planejamento.xlsx
+++ b/data/checks-planejamento.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B106"/>
+  <dimension ref="A1:B326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -373,72 +373,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>check_count_acoes_is_deleted</t>
+          <t>check_count_programas</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A ação 2500, uo 1261, consta como deletada na base ações-planejamento (desc.: ASSESSORAMENTO E ...) em inconsistência com a base localizadores (NA).</t>
+          <t>O programa 127 não consta na base localizadores, em detrimento das bases programas e ações-planejamento</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>check_count_acoes_is_deleted</t>
+          <t>check_count_acoes</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A ação 4161, uo 1321, consta como deletada na base ações-planejamento (desc.: VIGILÂNCIA DA ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 2106, uo 1251, consta na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>check_count_acoes_is_deleted</t>
+          <t>check_count_acoes</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A ação 4177, uo 1321, consta como deletada na base ações-planejamento (desc.: VIGILÂNCIA DA ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 4418, uo 1261, consta na base ações-planejamento (desc.: ESCOLA SEGURA ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>check_count_acoes_is_deleted</t>
+          <t>check_count_acoes</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A ação 1026, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 2103, uo 1401, consta na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>check_count_acoes_is_deleted</t>
+          <t>check_count_acoes</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A ação 1027, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 2104, uo 1401, consta na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>check_count_acoes_is_deleted</t>
+          <t>check_count_acoes</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A ação 1029, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 4411, uo 2311, consta na base ações-planejamento (desc.: GESTÃO DO ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A ação 1031, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 2108, uo 1251, consta como deletada na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
@@ -462,7 +462,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A ação 2417, uo 2421, consta como deletada na base ações-planejamento (desc.: REMUNERAÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 2500, uo 1261, consta como deletada na base ações-planejamento (desc.: ASSESSORAMENTO E ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A ação 2417, uo 2471, consta como deletada na base ações-planejamento (desc.: REMUNERAÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 4161, uo 1321, consta como deletada na base ações-planejamento (desc.: VIGILÂNCIA DA ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A ação 2500, uo 2471, consta como deletada na base ações-planejamento (desc.: ASSESSORAMENTO E ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 4177, uo 1321, consta como deletada na base ações-planejamento (desc.: VIGILÂNCIA DA ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
@@ -498,91 +498,91 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A ação 1034, uo 3041, consta como deletada na base ações-planejamento (desc.: MELHORAMENTO GENÉTICO ...) em inconsistência com a base localizadores (NA).</t>
+          <t>A ação 1026, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 10 está com os valores totais de receita e despesa diferentes nas bases. R$ 84.363.501.073,00 na base orçamento fiscal da receita, e 90.656.750.925,00 na qdd fiscal. A diferença é de R$ -6293249852.</t>
+          <t>A ação 1027, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 12 está com os valores totais de receita e despesa diferentes nas bases. R$ 444,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 444.</t>
+          <t>A ação 1029, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 20 está com os valores totais de receita e despesa diferentes nas bases. R$ 0,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ NA.</t>
+          <t>A ação 1031, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 31 está com os valores totais de receita e despesa diferentes nas bases. R$ 77.971.087,00 na base orçamento fiscal da receita, e 57.420.824,00 na qdd fiscal. A diferença é de R$ 20550263.</t>
+          <t>A ação 2417, uo 2421, consta como deletada na base ações-planejamento (desc.: REMUNERAÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 40 está com os valores totais de receita e despesa diferentes nas bases. R$ 392.059,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 392059.</t>
+          <t>A ação 2417, uo 2471, consta como deletada na base ações-planejamento (desc.: REMUNERAÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 46 está com os valores totais de receita e despesa diferentes nas bases. R$ 2.072,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 2072.</t>
+          <t>A ação 2500, uo 2471, consta como deletada na base ações-planejamento (desc.: ASSESSORAMENTO E ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 47 está com os valores totais de receita e despesa diferentes nas bases. R$ 28.687.328,00 na base orçamento fiscal da receita, e 14.640.082,00 na qdd fiscal. A diferença é de R$ 14047246.</t>
+          <t>A ação 1034, uo 3041, consta como deletada na base ações-planejamento (desc.: MELHORAMENTO GENÉTICO ...) em inconsistência com a base localizadores (NA).</t>
         </is>
       </c>
     </row>
@@ -594,7 +594,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 52 está com os valores totais de receita e despesa diferentes nas bases. R$ 52.340.332,00 na base orçamento fiscal da receita, e 24.743.178,00 na qdd fiscal. A diferença é de R$ 27597154.</t>
+          <t>A Fonte de Recurso 10 está com os valores totais de receita e despesa diferentes nas bases. R$ 84.363.501.073,00 na base orçamento fiscal da receita, e 90.656.750.925,00 na qdd fiscal. A diferença é de R$ -6293249852.</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 53 está com os valores totais de receita e despesa diferentes nas bases. R$ 1.600,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 1600.</t>
+          <t>A Fonte de Recurso 12 está com os valores totais de receita e despesa diferentes nas bases. R$ 444,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 444.</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 54 está com os valores totais de receita e despesa diferentes nas bases. R$ 6.682.512,00 na base orçamento fiscal da receita, e 4.104.010,00 na qdd fiscal. A diferença é de R$ 2578502.</t>
+          <t>A Fonte de Recurso 20 está com os valores totais de receita e despesa diferentes nas bases. R$ 0,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ NA.</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 59 está com os valores totais de receita e despesa diferentes nas bases. R$ 383.447.752,00 na base orçamento fiscal da receita, e 342.620.315,00 na qdd fiscal. A diferença é de R$ 40827437.</t>
+          <t>A Fonte de Recurso 31 está com os valores totais de receita e despesa diferentes nas bases. R$ 77.971.087,00 na base orçamento fiscal da receita, e 57.420.824,00 na qdd fiscal. A diferença é de R$ 20550263.</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 60 está com os valores totais de receita e despesa diferentes nas bases. R$ 4.528.328.118,00 na base orçamento fiscal da receita, e 3.795.212.436,00 na qdd fiscal. A diferença é de R$ 733115682.</t>
+          <t>A Fonte de Recurso 40 está com os valores totais de receita e despesa diferentes nas bases. R$ 392.059,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 392059.</t>
         </is>
       </c>
     </row>
@@ -654,7 +654,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 61 está com os valores totais de receita e despesa diferentes nas bases. R$ 433.782.405,00 na base orçamento fiscal da receita, e 406.710.026,00 na qdd fiscal. A diferença é de R$ 27072379.</t>
+          <t>A Fonte de Recurso 46 está com os valores totais de receita e despesa diferentes nas bases. R$ 2.072,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 2072.</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 72 está com os valores totais de receita e despesa diferentes nas bases. R$ 456.921.538,00 na base orçamento fiscal da receita, e 350.859.025,00 na qdd fiscal. A diferença é de R$ 106062513.</t>
+          <t>A Fonte de Recurso 47 está com os valores totais de receita e despesa diferentes nas bases. R$ 28.687.328,00 na base orçamento fiscal da receita, e 14.640.082,00 na qdd fiscal. A diferença é de R$ 14047246.</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 79 está com os valores totais de receita e despesa diferentes nas bases. R$ 7.765.658,00 na base orçamento fiscal da receita, e 4.000.000,00 na qdd fiscal. A diferença é de R$ 3765658.</t>
+          <t>A Fonte de Recurso 52 está com os valores totais de receita e despesa diferentes nas bases. R$ 52.340.332,00 na base orçamento fiscal da receita, e 24.743.178,00 na qdd fiscal. A diferença é de R$ 27597154.</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 83 está com os valores totais de receita e despesa diferentes nas bases. R$ 205.514.880,00 na base orçamento fiscal da receita, e 175.581.839,00 na qdd fiscal. A diferença é de R$ 29933041.</t>
+          <t>A Fonte de Recurso 53 está com os valores totais de receita e despesa diferentes nas bases. R$ 1.600,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 1600.</t>
         </is>
       </c>
     </row>
@@ -702,7 +702,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 91 está com os valores totais de receita e despesa diferentes nas bases. R$ 133.921.299,00 na base orçamento fiscal da receita, e 69.063.939,00 na qdd fiscal. A diferença é de R$ 64857360.</t>
+          <t>A Fonte de Recurso 54 está com os valores totais de receita e despesa diferentes nas bases. R$ 6.682.512,00 na base orçamento fiscal da receita, e 4.104.010,00 na qdd fiscal. A diferença é de R$ 2578502.</t>
         </is>
       </c>
     </row>
@@ -714,103 +714,103 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>A Fonte de Recurso 94 está com os valores totais de receita e despesa diferentes nas bases. R$ 10.715.576,00 na base orçamento fiscal da receita, e 6.760.698,00 na qdd fiscal. A diferença é de R$ 3954878.</t>
+          <t>A Fonte de Recurso 59 está com os valores totais de receita e despesa diferentes nas bases. R$ 383.447.752,00 na base orçamento fiscal da receita, e 342.620.315,00 na qdd fiscal. A diferença é de R$ 40827437.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_exists</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>O programa 2 contém indicador (PERCENTUAL DE INSTITUCIONALIZAÇÃO...) que, apesar de ter índice de referência de 100, está sem meta para o ano 0.</t>
+          <t>A Fonte de Recurso 60 está com os valores totais de receita e despesa diferentes nas bases. R$ 4.528.328.118,00 na base orçamento fiscal da receita, e 3.795.212.434,00 na qdd fiscal. A diferença é de R$ 733115684.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>O programa 3 contém indicador (ÍNDICE DE EFETIVIDADE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>A Fonte de Recurso 61 está com os valores totais de receita e despesa diferentes nas bases. R$ 433.782.405,00 na base orçamento fiscal da receita, e 406.710.026,00 na qdd fiscal. A diferença é de R$ 27072379.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>O programa 11 contém indicador (TAXA DE MATERIAIS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>A Fonte de Recurso 72 está com os valores totais de receita e despesa diferentes nas bases. R$ 456.921.538,00 na base orçamento fiscal da receita, e 350.859.025,00 na qdd fiscal. A diferença é de R$ 106062513.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>O programa 18 contém indicador (NUMERO DE MATÉRIAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>A Fonte de Recurso 79 está com os valores totais de receita e despesa diferentes nas bases. R$ 7.765.658,00 na base orçamento fiscal da receita, e 4.000.000,00 na qdd fiscal. A diferença é de R$ 3765658.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>O programa 27 contém indicador (EXECUÇÃO DAS METAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>A Fonte de Recurso 83 está com os valores totais de receita e despesa diferentes nas bases. R$ 205.514.880,00 na base orçamento fiscal da receita, e 175.581.839,00 na qdd fiscal. A diferença é de R$ 29933041.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>O programa 27 contém indicador (ABRANGÊNCIA DOS PROGRAMAS,...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>A Fonte de Recurso 91 está com os valores totais de receita e despesa diferentes nas bases. R$ 133.921.299,00 na base orçamento fiscal da receita, e 69.063.939,00 na qdd fiscal. A diferença é de R$ 64857360.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>O programa 27 contém indicador (INCREMENTO DE ABRANGÊNCIA...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>A Fonte de Recurso 94 está com os valores totais de receita e despesa diferentes nas bases. R$ 10.715.576,00 na base orçamento fiscal da receita, e 6.760.698,00 na qdd fiscal. A diferença é de R$ 3954878.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_indicadores_consistency_indice_de_referencia_exists</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>O programa 81 contém indicador (EVOLUÇÃO DA QUALIDADE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 2 contém indicador (PERCENTUAL DE INSTITUCIONALIZAÇÃO...) que, apesar de ter índice de referência de 100, está sem meta para o ano 0.</t>
         </is>
       </c>
     </row>
@@ -822,7 +822,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>O programa 91 contém indicador (DISCENTES FORMADOS E...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 3 contém indicador (ÍNDICE DE EFETIVIDADE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>O programa 91 contém indicador (ARTIGOS ACADÊMICOS ACEITOS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 11 contém indicador (TAXA DE MATERIAIS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>O programa 91 contém indicador (GRAU DE SATISFAÇÃO...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 18 contém indicador (NUMERO DE MATÉRIAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>O programa 99 contém indicador (ÍNDICE ACUMULADO DE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 27 contém indicador (INCREMENTO DE ABRANGÊNCIA...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>O programa 172 contém indicador (PERCENTUAL DE EXECUÇÃO...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 27 contém indicador (ABRANGÊNCIA DOS PROGRAMAS,...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -882,7 +882,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>O programa 172 contém indicador (PERCENTUAL DE OBRAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 27 contém indicador (EXECUÇÃO DAS METAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -894,7 +894,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>O programa 746 contém indicador (ÍNDICE DE IRREGULARIDADES...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 81 contém indicador (EVOLUÇÃO DA QUALIDADE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -906,103 +906,103 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>O programa 746 contém indicador (QUANTIDADE DE INDÍCIOS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+          <t>O programa 91 contém indicador (DISCENTES FORMADOS E...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>check_indicadores_justificativa_indice_referencia_em_apuracao</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>O programa 3 contém indicador (ÍNDICE DE EFETIVIDADE...) que está em apuração, porém com justificativa de status inválida, menos de 50 caracteres (43 caract. - O ÍNDICE SERÁ...).</t>
+          <t>O programa 91 contém indicador (GRAU DE SATISFAÇÃO...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>check_indicadores_justificativa_indice_referencia_em_apuracao</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>O programa 11 contém indicador (TAXA DE MATERIAIS...) que está em apuração, porém com justificativa de status inválida, menos de 50 caracteres (32 caract. - O ÍNDICE SERÁ...).</t>
+          <t>O programa 91 contém indicador (ARTIGOS ACADÊMICOS ACEITOS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>check_indicadores_justificativa_indice_referencia_em_apuracao</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>O programa 746 contém indicador (ÍNDICE DE IRREGULARIDADES...) que está em apuração, porém com justificativa de status inválida, menos de 50 caracteres (44 caract. - O PRIMEIRO EXERCÍCIO...).</t>
+          <t>O programa 99 contém indicador (ÍNDICE ACUMULADO DE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>check_indicadores_indice_referencia_data_futura</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>O programa 64 contém indicador (NÚMERO DE MUNICÍPIOS...) cujo índice de referência, apesar de não estar em apuração, apresenta data de apuração futura: 2025-12-31.</t>
+          <t>O programa 172 contém indicador (PERCENTUAL DE EXECUÇÃO...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>check_indicadores_previsoes_zeradas</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>O programa 92 contém indicador (TAXA DE EXPANSÃO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 172 contém indicador (PERCENTUAL DE OBRAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>check_indicadores_previsoes_zeradas</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>O programa 94 contém indicador (TAXA DE CRESCIMENTO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 746 contém indicador (QUANTIDADE DE INDÍCIOS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>check_indicadores_previsoes_zeradas</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>O programa 165 contém indicador (IDEB ANOS INICIAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 746 contém indicador (ÍNDICE DE IRREGULARIDADES...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>check_indicadores_previsoes_zeradas</t>
+          <t>check_indicadores_indice_referencia_data_futura</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>O programa 165 contém indicador (IDEB ENSINO MÉDIO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 64 contém indicador (NÚMERO DE MUNICÍPIOS...) cujo índice de referência, apesar de não estar em apuração, apresenta data de apuração futura: 2025-12-31.</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>O programa 165 contém indicador (IDEB ANOS FINAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 92 contém indicador (TAXA DE EXPANSÃO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>O programa 167 contém indicador (IDEB ANOS INICIAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 94 contém indicador (TAXA DE CRESCIMENTO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>O programa 167 contém indicador (IDEB ENSINO MÉDIO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 165 contém indicador (IDEB ANOS INICIAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -1050,55 +1050,55 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>O programa 167 contém indicador (IDEB ANOS FINAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+          <t>O programa 165 contém indicador (IDEB ENSINO MÉDIO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>check_intra_detalhamento</t>
+          <t>check_indicadores_previsoes_zeradas</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>A uo 1401 está com valor recebido de recursos intraorçamentários (R$ 960.756,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>O programa 165 contém indicador (IDEB ANOS FINAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>check_intra_detalhamento</t>
+          <t>check_indicadores_previsoes_zeradas</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>A uo 1451 está com valor recebido de recursos intraorçamentários (R$ 224.346.201,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>O programa 167 contém indicador (IDEB ANOS INICIAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>check_intra_detalhamento</t>
+          <t>check_indicadores_previsoes_zeradas</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>A uo 1541 está com valor recebido de recursos intraorçamentários (R$ 31.538.282,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>O programa 167 contém indicador (IDEB ENSINO MÉDIO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>check_intra_detalhamento</t>
+          <t>check_indicadores_previsoes_zeradas</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>A uo 2011 está com valor recebido de recursos intraorçamentários (R$ 647.702.182,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>O programa 167 contém indicador (IDEB ANOS FINAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>A uo 2121 está com valor recebido de recursos intraorçamentários (R$ 2.260.804.301,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 1401 está com valor recebido de recursos intraorçamentários (R$ 960.756,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>A uo 2251 está com valor recebido de recursos intraorçamentários (R$ 18.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 1451 está com valor recebido de recursos intraorçamentários (R$ 224.346.201,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>A uo 2261 está com valor recebido de recursos intraorçamentários (R$ 652.857.538,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 1541 está com valor recebido de recursos intraorçamentários (R$ 31.538.282,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>A uo 2271 está com valor recebido de recursos intraorçamentários (R$ 2.397.229.409,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 2011 está com valor recebido de recursos intraorçamentários (R$ 647.702.182,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>A uo 2321 está com valor recebido de recursos intraorçamentários (R$ 487.249.378,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 2121 está com valor recebido de recursos intraorçamentários (R$ 2.260.804.301,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>A uo 2361 está com valor recebido de recursos intraorçamentários (R$ 15.037.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 2251 está com valor recebido de recursos intraorçamentários (R$ 18.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>A uo 3051 está com valor recebido de recursos intraorçamentários (R$ 660.084,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 2261 está com valor recebido de recursos intraorçamentários (R$ 652.857.538,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>A uo 4031 está com valor recebido de recursos intraorçamentários (R$ 87.655.976,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 2271 está com valor recebido de recursos intraorçamentários (R$ 2.397.229.409,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>A uo 4631 está com valor recebido de recursos intraorçamentários (R$ 1.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 2321 está com valor recebido de recursos intraorçamentários (R$ 487.249.378,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>A uo 4661 está com valor recebido de recursos intraorçamentários (R$ 470.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 2361 está com valor recebido de recursos intraorçamentários (R$ 15.037.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>A uo 4711 está com valor recebido de recursos intraorçamentários (R$ 7.218.864.598,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 3051 está com valor recebido de recursos intraorçamentários (R$ 660.084,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1242,55 +1242,55 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>A uo 9901 está com valor recebido de recursos intraorçamentários (R$ 580.295.911,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+          <t>A uo 4031 está com valor recebido de recursos intraorçamentários (R$ 87.655.976,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>check_limite_ano0</t>
+          <t>check_intra_detalhamento</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>A uo 1231 está com uma diferença de R$ (15.387,00) entre o valor de limite no ano 0 (R$ 12.495.112,00) e a soma do valor utilizado no ano (R$ 12.510.499,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 12.510.499,00.</t>
+          <t>A uo 4631 está com valor recebido de recursos intraorçamentários (R$ 1.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>check_limite_ano0</t>
+          <t>check_intra_detalhamento</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>A uo 1301 está com uma diferença de R$ (1.000,00) entre o valor de limite no ano 0 (R$ 29.425.835,00) e a soma do valor utilizado no ano (R$ 29.426.835,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 29.426.835,00.</t>
+          <t>A uo 4661 está com valor recebido de recursos intraorçamentários (R$ 470.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>check_limite_ano0</t>
+          <t>check_intra_detalhamento</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>A uo 1451 está com uma diferença de R$ (150.714.182,00) entre o valor de limite no ano 0 (R$ 353.708.669,00) e a soma do valor utilizado no ano (R$ 504.422.851,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 504.422.851,00.</t>
+          <t>A uo 4711 está com valor recebido de recursos intraorçamentários (R$ 7.218.864.598,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>check_limite_ano0</t>
+          <t>check_intra_detalhamento</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>A uo 1451 está com uma diferença de R$ (1.778.147,00) entre o valor de limite no ano 0 (R$ 41.116.142,00) e a soma do valor utilizado no ano (R$ 42.894.289,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 42.894.289,00.</t>
+          <t>A uo 9901 está com valor recebido de recursos intraorçamentários (R$ 580.295.911,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>A uo 2171 está com uma diferença de R$ (2.000,00) entre o valor de limite no ano 0 (R$ 2.641.831,00) e a soma do valor utilizado no ano (R$ 2.643.831,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 2.643.831,00.</t>
+          <t>A uo 1231 está com uma diferença de R$ (15.387,00) entre o valor de limite no ano 0 (R$ 12.495.112,00) e a soma do valor utilizado no ano (R$ 12.510.499,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 12.510.499,00.</t>
         </is>
       </c>
     </row>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>A uo 2171 está com uma diferença de R$ (45.346,00) entre o valor de limite no ano 0 (R$ 1.145.946,00) e a soma do valor utilizado no ano (R$ 1.191.292,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 1.191.292,00.</t>
+          <t>A uo 1301 está com uma diferença de R$ (1.000,00) entre o valor de limite no ano 0 (R$ 29.425.835,00) e a soma do valor utilizado no ano (R$ 29.426.835,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 29.426.835,00.</t>
         </is>
       </c>
     </row>
@@ -1326,55 +1326,55 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>A uo 2371 está com uma diferença de R$ (26.250,00) entre o valor de limite no ano 0 (R$ 87.500,00) e a soma do valor utilizado no ano (R$ 113.750,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 113.750,00.</t>
+          <t>A uo 1451 está com uma diferença de R$ (150.714.182,00) entre o valor de limite no ano 0 (R$ 353.708.669,00) e a soma do valor utilizado no ano (R$ 504.422.851,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 504.422.851,00.</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>check_objetivos_estrategicos_exists</t>
+          <t>check_limite_ano0</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>O programa 98 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>A uo 1451 está com uma diferença de R$ (1.778.147,00) entre o valor de limite no ano 0 (R$ 41.116.142,00) e a soma do valor utilizado no ano (R$ 42.894.289,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 42.894.289,00.</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>check_objetivos_estrategicos_exists</t>
+          <t>check_limite_ano0</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>O programa 704 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>A uo 2171 está com uma diferença de R$ (2.000,00) entre o valor de limite no ano 0 (R$ 2.641.831,00) e a soma do valor utilizado no ano (R$ 2.643.831,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 2.643.831,00.</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>check_objetivos_estrategicos_exists</t>
+          <t>check_limite_ano0</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>O programa 706 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>A uo 2171 está com uma diferença de R$ (45.346,00) entre o valor de limite no ano 0 (R$ 1.145.946,00) e a soma do valor utilizado no ano (R$ 1.191.292,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 1.191.292,00.</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>check_objetivos_estrategicos_exists</t>
+          <t>check_limite_ano0</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>O programa 726 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>A uo 2371 está com uma diferença de R$ (26.250,00) entre o valor de limite no ano 0 (R$ 87.500,00) e a soma do valor utilizado no ano (R$ 113.750,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 113.750,00.</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>O programa 729 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 98 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>O programa 734 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 704 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>O programa 738 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 706 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>O programa 746 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 726 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>O programa 760 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 729 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>O programa 764 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 734 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>O programa 765 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 738 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>O programa 766 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 746 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
@@ -1482,103 +1482,103 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>O programa 767 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+          <t>O programa 760 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>check_ods_exists</t>
+          <t>check_objetivos_estrategicos_exists</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>O programa 126 está sem objetivo de desenvolvimento estratégico definido.</t>
+          <t>O programa 764 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>check_ods_exists</t>
+          <t>check_objetivos_estrategicos_exists</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>O programa 138 está sem objetivo de desenvolvimento estratégico definido.</t>
+          <t>O programa 765 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>check_setor_governo</t>
+          <t>check_objetivos_estrategicos_exists</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>A uo 1321 está com setor divergente na base ações-planejamento (SAÚDE) em relação à tabela auxiliar setor-governo da loa (NA).</t>
+          <t>O programa 766 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>check_setor_governo</t>
+          <t>check_objetivos_estrategicos_exists</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>A uo 1917 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (FAZENDA).</t>
+          <t>O programa 767 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>check_setor_governo</t>
+          <t>check_ods_exists</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>A uo 2471 está com setor divergente na base ações-planejamento (INFRAESTRUTURA, MOBILIDADE E PARCERIAS) em relação à tabela auxiliar setor-governo da loa (NA).</t>
+          <t>O programa 8 está sem objetivo de desenvolvimento estratégico definido.</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>check_setor_governo</t>
+          <t>check_ods_exists</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>A uo 4171 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (AGRICULTURA, PECUÁRIA E ABASTECIMENTO).</t>
+          <t>O programa 126 está sem objetivo de desenvolvimento estratégico definido.</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>check_setor_governo</t>
+          <t>check_ods_exists</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>A uo 4531 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (DESENVOLVIMENTO ECONÔMICO).</t>
+          <t>O programa 138 está sem objetivo de desenvolvimento estratégico definido.</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>check_setor_governo</t>
+          <t>check_ods_exists</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>A uo 4731 está com setor divergente na base ações-planejamento (MINISTÉRIO PÚBLICO) em relação à tabela auxiliar setor-governo da loa (NA).</t>
+          <t>O programa 142 está sem objetivo de desenvolvimento estratégico definido.</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>A uo 4741 está com setor divergente na base ações-planejamento (DEFENSORIA PÚBLICA) em relação à tabela auxiliar setor-governo da loa (NA).</t>
+          <t>A uo 1321 está com setor divergente na base ações-planejamento (SAÚDE) em relação à tabela auxiliar setor-governo da loa (NA).</t>
         </is>
       </c>
     </row>
@@ -1602,31 +1602,2674 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>A uo 4751 está com setor divergente na base ações-planejamento (ADVOCACIA GERAL) em relação à tabela auxiliar setor-governo da loa (NA).</t>
+          <t>A uo 1917 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (FAZENDA).</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>check_valores_qdd_fiscal</t>
+          <t>check_setor_governo</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>A uo 4031, programa 706, ação 4395, função 2, subfunção 61 está com valor na base qdd-fiscal (R$ 2.374.248.425,00) diferente da base ações-planejamento (R$ 2.374.248.423,00). Diferença de R$ 2.</t>
+          <t>A uo 4171 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (AGRICULTURA, PECUÁRIA E ABASTECIMENTO).</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>check_valores_qdd_plurianual</t>
+          <t>check_setor_governo</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>A uo 4031, programa 706, ação 4395, função 2, subfunção 61 está com valor do ano 0, base qdd-plurianual (R$ 2.374.248.425,00) diferente da base ações-planejamento (R$ 2.374.248.423,00). Diferença de R$ 2.</t>
+          <t>A uo 4531 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (DESENVOLVIMENTO ECONÔMICO).</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 127, ação 2106, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 127, ação 4418, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 127, ação 2104, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 165, ação 2103, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4411, função 10, subfunção 302, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_programas</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>A uo 2311, 
+programa 7, 
+área temática 03AT03 está com valor 
+de meta orçamentária do ano 0, base programas (R$ 187.558.168,00) diferente da base ações-planejamento (R$  NA). Diferença de R$ 187558168.</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 705, ação 2157, função 1, subfunção 32 está com valor na base qdd-fiscal (R$ 74.959.098,00) diferente da base ações-planejamento (R$ 86.343.439,00). Diferença de R$ -11384341.</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 705, ação 7006, função 9, subfunção 272 está com valor na base qdd-fiscal (R$ 538.964.784,00) diferente da base ações-planejamento (R$ 546.721.750,00). Diferença de R$ -7756966.</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 746, ação 2009, função 1, subfunção 122 está com valor na base qdd-fiscal (R$ 199.226.735,00) diferente da base ações-planejamento (R$ 202.637.401,00). Diferença de R$ -3410666.</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 760, ação 2145, função 1, subfunção 128 está com valor na base qdd-fiscal (R$ 8.462.193,00) diferente da base ações-planejamento (R$ 12.662.193,00). Diferença de R$ -4200000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>A uo 1071, programa 48, ação 4155, função 6, subfunção 182 está com valor na base qdd-fiscal (R$ 131.000,00) diferente da base ações-planejamento (R$ 1.731.000,00). Diferença de R$ -1600000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>A uo 1071, programa 101, ação 1008, função 6, subfunção 182 está com valor na base qdd-fiscal (R$ 14.800.970,00) diferente da base ações-planejamento (R$ 17.060.970,00). Diferença de R$ -2260000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>A uo 1221, programa 125, ação 1082, função 4, subfunção 127 está com valor na base qdd-fiscal (R$ 47.501.208,00) diferente da base ações-planejamento (R$ 48.281.208,00). Diferença de R$ -780000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>A uo 1221, programa 132, ação 4474, função 23, subfunção 691 está com valor na base qdd-fiscal (R$ 617.333,00) diferente da base ações-planejamento (R$ 1.117.333,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 108, ação 4358, função 20, subfunção 608 está com valor na base qdd-fiscal (R$ 9.441.948,00) diferente da base ações-planejamento (R$ 11.326.448,00). Diferença de R$ -1884500.</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 110, ação 4363, função 21, subfunção 605 está com valor na base qdd-fiscal (R$ 8.311.853,00) diferente da base ações-planejamento (R$ 9.061.853,00). Diferença de R$ -750000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 111, ação 4383, função 20, subfunção 608 está com valor na base qdd-fiscal (R$ 13.387.942,00) diferente da base ações-planejamento (R$ 13.537.942,00). Diferença de R$ -150000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 111, ação 4420, função 20, subfunção 608 está com valor na base qdd-fiscal (R$ 30.000.000,00) diferente da base ações-planejamento (R$ 53.592.878,00). Diferença de R$ -23592878.</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 112, ação 4403, função 20, subfunção 608 está com valor na base qdd-fiscal (R$ 5.720.025,00) diferente da base ações-planejamento (R$ 5.810.235,00). Diferença de R$ -90210.</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 114, ação 4398, função 20, subfunção 607 está com valor na base qdd-fiscal (R$ 11.866.753,00) diferente da base ações-planejamento (R$ 13.841.359,00). Diferença de R$ -1974606.</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 114, ação 4419, função 20, subfunção 127 está com valor na base qdd-fiscal (R$ 1.377.192,00) diferente da base ações-planejamento (R$ 2.377.192,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 705, ação 2500, função 20, subfunção 122 está com valor na base qdd-fiscal (R$ 12.430.883,00) diferente da base ações-planejamento (R$ 13.930.883,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 127, ação 2106, função 12, subfunção 368 está com valor na base qdd-fiscal (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4365, função 6, subfunção 181 está com valor na base qdd-fiscal (R$ 6.334.166.724,00) diferente da base ações-planejamento (R$ 6.334.866.724,00). Diferença de R$ -7e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4366, função 6, subfunção 181 está com valor na base qdd-fiscal (R$ 1.050,00) diferente da base ações-planejamento (R$ 40.343.178,00). Diferença de R$ -40342128.</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4373, função 6, subfunção 181 está com valor na base qdd-fiscal (R$ 3.600,00) diferente da base ações-planejamento (R$ 103.600,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 705, ação 2500, função 6, subfunção 122 está com valor na base qdd-fiscal (R$ 376.861.077,00) diferente da base ações-planejamento (R$ 378.361.077,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 127, ação 4418, função 12, subfunção 368 está com valor na base qdd-fiscal (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 167, ação 2122, função 12, subfunção 361 está com valor na base qdd-fiscal (R$ 117.100.000,00) diferente da base ações-planejamento (R$ 118.550.000,00). Diferença de R$ -1450000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 167, ação 4511, função 12, subfunção 362 está com valor na base qdd-fiscal (R$ 62.600.000,00) diferente da base ações-planejamento (R$ 66.600.000,00). Diferença de R$ -4e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 2126, função 12, subfunção 368 está com valor na base qdd-fiscal (R$ 456.147.344,00) diferente da base ações-planejamento (R$ 553.858.039,00). Diferença de R$ -97710695.</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 4519, função 12, subfunção 368 está com valor na base qdd-fiscal (R$ 524.704.215,00) diferente da base ações-planejamento (R$ 534.715.902,00). Diferença de R$ -10011687.</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 4527, função 12, subfunção 368 está com valor na base qdd-fiscal (R$ 644.976.000,00) diferente da base ações-planejamento (R$ 650.592.317,00). Diferença de R$ -5616317.</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 172, ação 4545, função 12, subfunção 361 está com valor na base qdd-fiscal (R$ 45.000.000,00) diferente da base ações-planejamento (R$ 45.324.049,00). Diferença de R$ -324049.</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 102, ação 4332, função 13, subfunção 392 está com valor na base qdd-fiscal (R$ 33.144.232,00) diferente da base ações-planejamento (R$ 49.994.232,00). Diferença de R$ -16850000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 102, ação 4343, função 13, subfunção 392 está com valor na base qdd-fiscal (R$ 170.568.000,00) diferente da base ações-planejamento (R$ 170.569.000,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 103, ação 4322, função 13, subfunção 392 está com valor na base qdd-fiscal (R$ 10.500.000,00) diferente da base ações-planejamento (R$ 10.800.000,00). Diferença de R$ -3e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 705, ação 2500, função 13, subfunção 122 está com valor na base qdd-fiscal (R$ 2.820.327,00) diferente da base ações-planejamento (R$ 3.320.327,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>A uo 1301, programa 99, ação 4261, função 15, subfunção 451 está com valor na base qdd-fiscal (R$ 7.140.411,00) diferente da base ações-planejamento (R$ 10.140.411,00). Diferença de R$ -3e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>A uo 1301, programa 99, ação 4262, função 15, subfunção 451 está com valor na base qdd-fiscal (R$ 16.016.092,00) diferente da base ações-planejamento (R$ 35.016.092,00). Diferença de R$ -1.9e+07.</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 21, ação 4028, função 17, subfunção 512 está com valor na base qdd-fiscal (R$ 50.231.475,00) diferente da base ações-planejamento (R$ 51.439.475,00). Diferença de R$ -1208000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 21, ação 4044, função 17, subfunção 512 está com valor na base qdd-fiscal (R$ 3.819.644,00) diferente da base ações-planejamento (R$ 4.219.644,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4045, função 18, subfunção 541 está com valor na base qdd-fiscal (R$ 807.634,00) diferente da base ações-planejamento (R$ 2.807.634,00). Diferença de R$ -2e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4046, função 18, subfunção 541 está com valor na base qdd-fiscal (R$ 557.957,00) diferente da base ações-planejamento (R$ 558.957,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4047, função 18, subfunção 541 está com valor na base qdd-fiscal (R$ 685.640,00) diferente da base ações-planejamento (R$ 34.385.640,00). Diferença de R$ -33700000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4124, função 18, subfunção 541 está com valor na base qdd-fiscal (R$ 4.000.000,00) diferente da base ações-planejamento (R$ 4.800.000,00). Diferença de R$ -8e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4114, função 6, subfunção 182 está com valor na base qdd-fiscal (R$ 486.636.314,00) diferente da base ações-planejamento (R$ 494.723.314,00). Diferença de R$ -8087000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4115, função 6, subfunção 182 está com valor na base qdd-fiscal (R$ 687.674.923,00) diferente da base ações-planejamento (R$ 688.174.923,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4120, função 6, subfunção 182 está com valor na base qdd-fiscal (R$ 11.030.599,00) diferente da base ações-planejamento (R$ 14.160.599,00). Diferença de R$ -3130000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4138, função 18, subfunção 182 está com valor na base qdd-fiscal (R$ 11.690.903,00) diferente da base ações-planejamento (R$ 12.690.903,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 53, ação 4094, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 960.756,00) diferente da base ações-planejamento (R$ 8.281.747,00). Diferença de R$ -7320991.</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 127, ação 2104, função 12, subfunção 368 está com valor na base qdd-fiscal (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 165, ação 2103, função 12, subfunção 368 está com valor na base qdd-fiscal (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>A uo 1441, programa 705, ação 7006, função 9, subfunção 272 está com valor na base qdd-fiscal (R$ 181.823.806,00) diferente da base ações-planejamento (R$ 186.703.806,00). Diferença de R$ -4880000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>A uo 1441, programa 726, ação 4193, função 3, subfunção 92 está com valor na base qdd-fiscal (R$ 855.538.836,00) diferente da base ações-planejamento (R$ 865.658.836,00). Diferença de R$ -10120000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 129, ação 4344, função 6, subfunção 421 está com valor na base qdd-fiscal (R$ 51.978.801,00) diferente da base ações-planejamento (R$ 52.679.791,00). Diferença de R$ -700990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 129, ação 4347, função 6, subfunção 421 está com valor na base qdd-fiscal (R$ 2.002.000,00) diferente da base ações-planejamento (R$ 2.003.000,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 1048, função 6, subfunção 421 está com valor na base qdd-fiscal (R$ 58.811.637,00) diferente da base ações-planejamento (R$ 63.784.579,00). Diferença de R$ -4972942.</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 4348, função 6, subfunção 421 está com valor na base qdd-fiscal (R$ 735.242.265,00) diferente da base ações-planejamento (R$ 736.174.265,00). Diferença de R$ -932000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 4351, função 6, subfunção 421 está com valor na base qdd-fiscal (R$ 124.967.835,00) diferente da base ações-planejamento (R$ 125.067.835,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 141, ação 4438, função 6, subfunção 422 está com valor na base qdd-fiscal (R$ 6.775.354,00) diferente da base ações-planejamento (R$ 7.275.354,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 66, ação 4153, função 11, subfunção 334 está com valor na base qdd-fiscal (R$ 6.876.017,00) diferente da base ações-planejamento (R$ 7.126.017,00). Diferença de R$ -250000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4167, função 27, subfunção 812 está com valor na base qdd-fiscal (R$ 1.187.363,00) diferente da base ações-planejamento (R$ 1.687.363,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4170, função 27, subfunção 812 está com valor na base qdd-fiscal (R$ 1.374.510,00) diferente da base ações-planejamento (R$ 11.159.340,00). Diferença de R$ -9784830.</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4514, função 27, subfunção 812 está com valor na base qdd-fiscal (R$ 3.378.169,00) diferente da base ações-planejamento (R$ 3.628.169,00). Diferença de R$ -250000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 70, ação 4174, função 14, subfunção 422 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$ 2.001.990,00). Diferença de R$ -2000990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 74, ação 4196, função 14, subfunção 306 está com valor na base qdd-fiscal (R$ 1.242.678,00) diferente da base ações-planejamento (R$ 1.642.678,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 86, ação 4415, função 14, subfunção 422 está com valor na base qdd-fiscal (R$ 2.622.178,00) diferente da base ações-planejamento (R$ 2.722.178,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 148, ação 2079, função 4, subfunção 122 está com valor na base qdd-fiscal (R$ 5.634.602,00) diferente da base ações-planejamento (R$ 16.425.592,00). Diferença de R$ -10790990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>A uo 1491, programa 119, ação 2045, função 4, subfunção 122 está com valor na base qdd-fiscal (R$ 3.189.678,00) diferente da base ações-planejamento (R$ 98.946.739,00). Diferença de R$ -95757061.</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>A uo 1491, programa 119, ação 2048, função 4, subfunção 122 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$ 861.067.452,00). Diferença de R$ -861066452.</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>A uo 1501, programa 156, ação 4465, função 4, subfunção 122 está com valor na base qdd-fiscal (R$ 95.680.170,00) diferente da base ações-planejamento (R$ 96.243.170,00). Diferença de R$ -563000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 1006, função 6, subfunção 181 está com valor na base qdd-fiscal (R$ 316,00) diferente da base ações-planejamento (R$ 500.316,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 1007, função 6, subfunção 181 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$ 21.138.490,00). Diferença de R$ -21137490.</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 4060, função 6, subfunção 181 está com valor na base qdd-fiscal (R$ 158.599.650,00) diferente da base ações-planejamento (R$ 161.249.650,00). Diferença de R$ -2650000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 4061, função 6, subfunção 181 está com valor na base qdd-fiscal (R$ 14.695.363,00) diferente da base ações-planejamento (R$ 14.845.363,00). Diferença de R$ -150000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>A uo 2071, programa 22, ação 4513, função 19, subfunção 571 está com valor na base qdd-fiscal (R$ 182.314.608,00) diferente da base ações-planejamento (R$ 182.514.607,00). Diferença de R$ -199999.</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>A uo 2101, programa 31, ação 4056, função 18, subfunção 543 está com valor na base qdd-fiscal (R$ 26.736.707,00) diferente da base ações-planejamento (R$ 27.136.707,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>A uo 2101, programa 31, ação 4059, função 18, subfunção 541 está com valor na base qdd-fiscal (R$ 55.956.871,00) diferente da base ações-planejamento (R$ 57.356.871,00). Diferença de R$ -1400000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>A uo 2201, programa 106, ação 4276, função 13, subfunção 391 está com valor na base qdd-fiscal (R$ 63.050,00) diferente da base ações-planejamento (R$ 598.050,00). Diferença de R$ -535000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>A uo 2201, programa 106, ação 4278, função 13, subfunção 391 está com valor na base qdd-fiscal (R$ 848.458,00) diferente da base ações-planejamento (R$ 1.348.458,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>A uo 2271, programa 19, ação 4031, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 403.048.770,00) diferente da base ações-planejamento (R$ 403.408.770,00). Diferença de R$ -360000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>A uo 2271, programa 19, ação 4036, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 203.935.708,00) diferente da base ações-planejamento (R$ 204.475.708,00). Diferença de R$ -540000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4268, função 26, subfunção 782 está com valor na base qdd-fiscal (R$ 88.091.501,00) diferente da base ações-planejamento (R$ 88.092.501,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4275, função 26, subfunção 782 está com valor na base qdd-fiscal (R$ 363.158.594,00) diferente da base ações-planejamento (R$ 363.159.594,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4293, função 26, subfunção 782 está com valor na base qdd-fiscal (R$ 651.192.418,00) diferente da base ações-planejamento (R$ 651.193.418,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4002, função 12, subfunção 364 está com valor na base qdd-fiscal (R$ 3.958.056,00) diferente da base ações-planejamento (R$ 5.458.056,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4005, função 12, subfunção 364 está com valor na base qdd-fiscal (R$ 4.525.088,00) diferente da base ações-planejamento (R$ 9.525.088,00). Diferença de R$ -5e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4411, função 10, subfunção 302 está com valor na base qdd-fiscal (R$  NA) diferente da base ações-planejamento (R$  NA). Diferença de R$ NA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 705, ação 2500, função 12, subfunção 122 está com valor na base qdd-fiscal (R$ 10.931.901,00) diferente da base ações-planejamento (R$ 11.431.901,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4086, função 12, subfunção 364 está com valor na base qdd-fiscal (R$ 115.679.715,00) diferente da base ações-planejamento (R$ 117.379.715,00). Diferença de R$ -1700000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4087, função 12, subfunção 364 está com valor na base qdd-fiscal (R$ 5.959.778,00) diferente da base ações-planejamento (R$ 5.960.778,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4089, função 12, subfunção 364 está com valor na base qdd-fiscal (R$ 6.377.753,00) diferente da base ações-planejamento (R$ 10.977.753,00). Diferença de R$ -4600000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4090, função 12, subfunção 364 está com valor na base qdd-fiscal (R$ 24.069.722,00) diferente da base ações-planejamento (R$ 24.909.722,00). Diferença de R$ -840000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 101, ação 1016, função 8, subfunção 544 está com valor na base qdd-fiscal (R$ 4.842.287,00) diferente da base ações-planejamento (R$ 5.957.287,00). Diferença de R$ -1115000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 101, ação 1032, função 8, subfunção 544 está com valor na base qdd-fiscal (R$ 3.206.136,00) diferente da base ações-planejamento (R$ 9.447.126,00). Diferença de R$ -6240990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 124, ação 4325, função 20, subfunção 608 está com valor na base qdd-fiscal (R$ 648.218,00) diferente da base ações-planejamento (R$ 1.048.218,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 124, ação 4516, função 20, subfunção 608 está com valor na base qdd-fiscal (R$ 411.620,00) diferente da base ações-planejamento (R$ 3.911.620,00). Diferença de R$ -3500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 90, ação 4235, função 20, subfunção 606 está com valor na base qdd-fiscal (R$ 92.806.224,00) diferente da base ações-planejamento (R$ 95.106.224,00). Diferença de R$ -2300000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 97, ação 4236, função 20, subfunção 608 está com valor na base qdd-fiscal (R$ 58.536.458,00) diferente da base ações-planejamento (R$ 78.162.208,00). Diferença de R$ -19625750.</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 705, ação 2500, função 20, subfunção 122 está com valor na base qdd-fiscal (R$ 1.744.815,00) diferente da base ações-planejamento (R$ 2.244.815,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>A uo 3051, programa 16, ação 4018, função 19, subfunção 571 está com valor na base qdd-fiscal (R$ 31.454.979,00) diferente da base ações-planejamento (R$ 31.564.979,00). Diferença de R$ -110000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>A uo 4251, programa 71, ação 2074, função 8, subfunção 244 está com valor na base qdd-fiscal (R$ 213.000,00) diferente da base ações-planejamento (R$ 1.213.000,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 58, ação 4121, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 2.432.886.227,00) diferente da base ações-planejamento (R$ 2.652.501.397,00). Diferença de R$ -219615170.</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 58, ação 4123, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 213.825.175,00) diferente da base ações-planejamento (R$ 267.869.644,00). Diferença de R$ -54044469.</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 60, ação 4125, função 10, subfunção 301 está com valor na base qdd-fiscal (R$ 449.100.000,00) diferente da base ações-planejamento (R$ 1.038.756.948,00). Diferença de R$ -589656948.</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 60, ação 4127, função 10, subfunção 301 está com valor na base qdd-fiscal (R$ 135.732.206,00) diferente da base ações-planejamento (R$ 332.118.192,00). Diferença de R$ -196385986.</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 61, ação 4129, função 10, subfunção 242 está com valor na base qdd-fiscal (R$ 218.709.539,00) diferente da base ações-planejamento (R$ 221.549.539,00). Diferença de R$ -2840000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 61, ação 4130, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 122.691.215,00) diferente da base ações-planejamento (R$ 126.051.462,00). Diferença de R$ -3360247.</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 61, ação 4131, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 364.234.946,00) diferente da base ações-planejamento (R$ 367.234.946,00). Diferença de R$ -3e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 62, ação 4135, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 1.255.000,00) diferente da base ações-planejamento (R$ 25.261.085,00). Diferença de R$ -24006085.</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 705, ação 2500, função 10, subfunção 122 está com valor na base qdd-fiscal (R$ 261.990.084,00) diferente da base ações-planejamento (R$ 303.872.066,00). Diferença de R$ -41881982.</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>A uo 4491, programa 102, ação 4360, função 13, subfunção 392 está com valor na base qdd-fiscal (R$ 31.999.000,00) diferente da base ações-planejamento (R$ 32.999.000,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 705, ação 2157, função 1, subfunção 32 está com valor do ano 0, base qdd-plurianual (R$ 74.959.098,00) diferente da base ações-planejamento (R$ 86.343.439,00). Diferença de R$ -11384341.</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 705, ação 7006, função 9, subfunção 272 está com valor do ano 0, base qdd-plurianual (R$ 538.964.784,00) diferente da base ações-planejamento (R$ 546.721.750,00). Diferença de R$ -7756966.</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 746, ação 2009, função 1, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 199.226.735,00) diferente da base ações-planejamento (R$ 202.637.401,00). Diferença de R$ -3410666.</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 760, ação 2145, função 1, subfunção 128 está com valor do ano 0, base qdd-plurianual (R$ 8.462.193,00) diferente da base ações-planejamento (R$ 12.662.193,00). Diferença de R$ -4200000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>A uo 1071, programa 48, ação 4155, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 131.000,00) diferente da base ações-planejamento (R$ 1.731.000,00). Diferença de R$ -1600000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>A uo 1071, programa 101, ação 1008, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 14.800.970,00) diferente da base ações-planejamento (R$ 17.060.970,00). Diferença de R$ -2260000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>A uo 1221, programa 125, ação 1082, função 4, subfunção 127 está com valor do ano 0, base qdd-plurianual (R$ 47.501.208,00) diferente da base ações-planejamento (R$ 48.281.208,00). Diferença de R$ -780000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>A uo 1221, programa 132, ação 4474, função 23, subfunção 691 está com valor do ano 0, base qdd-plurianual (R$ 617.333,00) diferente da base ações-planejamento (R$ 1.117.333,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 108, ação 4358, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 9.441.948,00) diferente da base ações-planejamento (R$ 11.326.448,00). Diferença de R$ -1884500.</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 110, ação 4363, função 21, subfunção 605 está com valor do ano 0, base qdd-plurianual (R$ 8.311.853,00) diferente da base ações-planejamento (R$ 9.061.853,00). Diferença de R$ -750000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 111, ação 4383, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 13.387.942,00) diferente da base ações-planejamento (R$ 13.537.942,00). Diferença de R$ -150000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 111, ação 4420, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 30.000.000,00) diferente da base ações-planejamento (R$ 53.592.878,00). Diferença de R$ -23592878.</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 112, ação 4403, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 5.720.025,00) diferente da base ações-planejamento (R$ 5.810.235,00). Diferença de R$ -90210.</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 114, ação 4398, função 20, subfunção 607 está com valor do ano 0, base qdd-plurianual (R$ 11.866.753,00) diferente da base ações-planejamento (R$ 13.841.359,00). Diferença de R$ -1974606.</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 114, ação 4419, função 20, subfunção 127 está com valor do ano 0, base qdd-plurianual (R$ 1.377.192,00) diferente da base ações-planejamento (R$ 2.377.192,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 705, ação 2500, função 20, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 12.430.883,00) diferente da base ações-planejamento (R$ 13.930.883,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 127, ação 2106, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4365, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 6.334.166.724,00) diferente da base ações-planejamento (R$ 6.334.866.724,00). Diferença de R$ -7e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4366, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 1.050,00) diferente da base ações-planejamento (R$ 40.343.178,00). Diferença de R$ -40342128.</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4373, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 3.600,00) diferente da base ações-planejamento (R$ 103.600,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 705, ação 2500, função 6, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 376.861.077,00) diferente da base ações-planejamento (R$ 378.361.077,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 127, ação 4418, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 167, ação 2122, função 12, subfunção 361 está com valor do ano 0, base qdd-plurianual (R$ 117.100.000,00) diferente da base ações-planejamento (R$ 118.550.000,00). Diferença de R$ -1450000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 167, ação 4511, função 12, subfunção 362 está com valor do ano 0, base qdd-plurianual (R$ 62.600.000,00) diferente da base ações-planejamento (R$ 66.600.000,00). Diferença de R$ -4e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 2126, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$ 456.147.344,00) diferente da base ações-planejamento (R$ 553.858.039,00). Diferença de R$ -97710695.</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 4519, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$ 524.704.215,00) diferente da base ações-planejamento (R$ 534.715.902,00). Diferença de R$ -10011687.</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 4527, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$ 644.976.000,00) diferente da base ações-planejamento (R$ 650.592.317,00). Diferença de R$ -5616317.</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 172, ação 4545, função 12, subfunção 361 está com valor do ano 0, base qdd-plurianual (R$ 45.000.000,00) diferente da base ações-planejamento (R$ 45.324.049,00). Diferença de R$ -324049.</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 102, ação 4332, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 33.144.232,00) diferente da base ações-planejamento (R$ 49.994.232,00). Diferença de R$ -16850000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 102, ação 4343, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 170.568.000,00) diferente da base ações-planejamento (R$ 170.569.000,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 103, ação 4322, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 10.500.000,00) diferente da base ações-planejamento (R$ 10.800.000,00). Diferença de R$ -3e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 705, ação 2500, função 13, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 2.820.327,00) diferente da base ações-planejamento (R$ 3.320.327,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>A uo 1301, programa 99, ação 4261, função 15, subfunção 451 está com valor do ano 0, base qdd-plurianual (R$ 7.140.411,00) diferente da base ações-planejamento (R$ 10.140.411,00). Diferença de R$ -3e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>A uo 1301, programa 99, ação 4262, função 15, subfunção 451 está com valor do ano 0, base qdd-plurianual (R$ 16.016.092,00) diferente da base ações-planejamento (R$ 35.016.092,00). Diferença de R$ -1.9e+07.</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 21, ação 4028, função 17, subfunção 512 está com valor do ano 0, base qdd-plurianual (R$ 50.231.475,00) diferente da base ações-planejamento (R$ 51.439.475,00). Diferença de R$ -1208000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 21, ação 4044, função 17, subfunção 512 está com valor do ano 0, base qdd-plurianual (R$ 3.819.644,00) diferente da base ações-planejamento (R$ 4.219.644,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4045, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 807.634,00) diferente da base ações-planejamento (R$ 2.807.634,00). Diferença de R$ -2e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4046, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 557.957,00) diferente da base ações-planejamento (R$ 558.957,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4047, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 685.640,00) diferente da base ações-planejamento (R$ 34.385.640,00). Diferença de R$ -33700000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4124, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 4.000.000,00) diferente da base ações-planejamento (R$ 4.800.000,00). Diferença de R$ -8e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4114, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 486.636.314,00) diferente da base ações-planejamento (R$ 494.723.314,00). Diferença de R$ -8087000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4115, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 687.674.923,00) diferente da base ações-planejamento (R$ 688.174.923,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4120, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 11.030.599,00) diferente da base ações-planejamento (R$ 14.160.599,00). Diferença de R$ -3130000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4138, função 18, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 11.690.903,00) diferente da base ações-planejamento (R$ 12.690.903,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 53, ação 4094, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 960.756,00) diferente da base ações-planejamento (R$ 8.281.747,00). Diferença de R$ -7320991.</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 127, ação 2104, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 165, ação 2103, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>A uo 1441, programa 705, ação 7006, função 9, subfunção 272 está com valor do ano 0, base qdd-plurianual (R$ 181.823.806,00) diferente da base ações-planejamento (R$ 186.703.806,00). Diferença de R$ -4880000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>A uo 1441, programa 726, ação 4193, função 3, subfunção 92 está com valor do ano 0, base qdd-plurianual (R$ 855.538.836,00) diferente da base ações-planejamento (R$ 865.658.836,00). Diferença de R$ -10120000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 129, ação 4344, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 51.978.801,00) diferente da base ações-planejamento (R$ 52.679.791,00). Diferença de R$ -700990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 129, ação 4347, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 2.002.000,00) diferente da base ações-planejamento (R$ 2.003.000,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 1048, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 58.811.637,00) diferente da base ações-planejamento (R$ 63.784.579,00). Diferença de R$ -4972942.</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 4348, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 735.242.265,00) diferente da base ações-planejamento (R$ 736.174.265,00). Diferença de R$ -932000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 4351, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 124.967.835,00) diferente da base ações-planejamento (R$ 125.067.835,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 141, ação 4438, função 6, subfunção 422 está com valor do ano 0, base qdd-plurianual (R$ 6.775.354,00) diferente da base ações-planejamento (R$ 7.275.354,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 66, ação 4153, função 11, subfunção 334 está com valor do ano 0, base qdd-plurianual (R$ 6.876.017,00) diferente da base ações-planejamento (R$ 7.126.017,00). Diferença de R$ -250000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4167, função 27, subfunção 812 está com valor do ano 0, base qdd-plurianual (R$ 1.187.363,00) diferente da base ações-planejamento (R$ 1.687.363,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4170, função 27, subfunção 812 está com valor do ano 0, base qdd-plurianual (R$ 1.374.510,00) diferente da base ações-planejamento (R$ 11.159.340,00). Diferença de R$ -9784830.</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4514, função 27, subfunção 812 está com valor do ano 0, base qdd-plurianual (R$ 3.378.169,00) diferente da base ações-planejamento (R$ 3.628.169,00). Diferença de R$ -250000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 70, ação 4174, função 14, subfunção 422 está com valor do ano 0, base qdd-plurianual (R$ 1.000,00) diferente da base ações-planejamento (R$ 2.001.990,00). Diferença de R$ -2000990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 74, ação 4196, função 14, subfunção 306 está com valor do ano 0, base qdd-plurianual (R$ 1.242.678,00) diferente da base ações-planejamento (R$ 1.642.678,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 86, ação 4415, função 14, subfunção 422 está com valor do ano 0, base qdd-plurianual (R$ 2.622.178,00) diferente da base ações-planejamento (R$ 2.722.178,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 148, ação 2079, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 5.634.602,00) diferente da base ações-planejamento (R$ 16.425.592,00). Diferença de R$ -10790990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>A uo 1491, programa 119, ação 2045, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 3.189.678,00) diferente da base ações-planejamento (R$ 98.946.739,00). Diferença de R$ -95757061.</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>A uo 1491, programa 119, ação 2048, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 1.000,00) diferente da base ações-planejamento (R$ 861.067.452,00). Diferença de R$ -861066452.</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>A uo 1501, programa 156, ação 4465, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 95.680.170,00) diferente da base ações-planejamento (R$ 96.243.170,00). Diferença de R$ -563000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 1006, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 316,00) diferente da base ações-planejamento (R$ 500.316,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 1007, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 1.000,00) diferente da base ações-planejamento (R$ 21.138.490,00). Diferença de R$ -21137490.</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 4060, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 158.599.650,00) diferente da base ações-planejamento (R$ 161.249.650,00). Diferença de R$ -2650000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 4061, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 14.695.363,00) diferente da base ações-planejamento (R$ 14.845.363,00). Diferença de R$ -150000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>A uo 2071, programa 22, ação 4513, função 19, subfunção 571 está com valor do ano 0, base qdd-plurianual (R$ 182.314.608,00) diferente da base ações-planejamento (R$ 182.514.607,00). Diferença de R$ -199999.</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>A uo 2101, programa 31, ação 4056, função 18, subfunção 543 está com valor do ano 0, base qdd-plurianual (R$ 26.736.707,00) diferente da base ações-planejamento (R$ 27.136.707,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>A uo 2101, programa 31, ação 4059, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 55.956.871,00) diferente da base ações-planejamento (R$ 57.356.871,00). Diferença de R$ -1400000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>A uo 2201, programa 106, ação 4276, função 13, subfunção 391 está com valor do ano 0, base qdd-plurianual (R$ 63.050,00) diferente da base ações-planejamento (R$ 598.050,00). Diferença de R$ -535000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>A uo 2201, programa 106, ação 4278, função 13, subfunção 391 está com valor do ano 0, base qdd-plurianual (R$ 848.458,00) diferente da base ações-planejamento (R$ 1.348.458,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>A uo 2271, programa 19, ação 4031, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 403.048.770,00) diferente da base ações-planejamento (R$ 403.408.770,00). Diferença de R$ -360000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>A uo 2271, programa 19, ação 4036, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 203.935.708,00) diferente da base ações-planejamento (R$ 204.475.708,00). Diferença de R$ -540000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4268, função 26, subfunção 782 está com valor do ano 0, base qdd-plurianual (R$ 88.091.501,00) diferente da base ações-planejamento (R$ 88.092.501,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4275, função 26, subfunção 782 está com valor do ano 0, base qdd-plurianual (R$ 363.158.594,00) diferente da base ações-planejamento (R$ 363.159.594,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4293, função 26, subfunção 782 está com valor do ano 0, base qdd-plurianual (R$ 651.192.418,00) diferente da base ações-planejamento (R$ 651.193.418,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4002, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 3.958.056,00) diferente da base ações-planejamento (R$ 5.458.056,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4005, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 4.525.088,00) diferente da base ações-planejamento (R$ 9.525.088,00). Diferença de R$ -5e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4411, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$  NA). Diferença de R$ NA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 705, ação 2500, função 12, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 10.931.901,00) diferente da base ações-planejamento (R$ 11.431.901,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4086, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 115.679.715,00) diferente da base ações-planejamento (R$ 117.379.715,00). Diferença de R$ -1700000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4087, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 5.959.778,00) diferente da base ações-planejamento (R$ 5.960.778,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4089, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 6.377.753,00) diferente da base ações-planejamento (R$ 10.977.753,00). Diferença de R$ -4600000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4090, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 24.069.722,00) diferente da base ações-planejamento (R$ 24.909.722,00). Diferença de R$ -840000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 101, ação 1016, função 8, subfunção 544 está com valor do ano 0, base qdd-plurianual (R$ 4.842.287,00) diferente da base ações-planejamento (R$ 5.957.287,00). Diferença de R$ -1115000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 101, ação 1032, função 8, subfunção 544 está com valor do ano 0, base qdd-plurianual (R$ 3.206.136,00) diferente da base ações-planejamento (R$ 9.447.126,00). Diferença de R$ -6240990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 124, ação 4325, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 648.218,00) diferente da base ações-planejamento (R$ 1.048.218,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 124, ação 4516, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 411.620,00) diferente da base ações-planejamento (R$ 3.911.620,00). Diferença de R$ -3500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 90, ação 4235, função 20, subfunção 606 está com valor do ano 0, base qdd-plurianual (R$ 92.806.224,00) diferente da base ações-planejamento (R$ 95.106.224,00). Diferença de R$ -2300000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 97, ação 4236, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 58.536.458,00) diferente da base ações-planejamento (R$ 78.162.208,00). Diferença de R$ -19625750.</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 705, ação 2500, função 20, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 1.744.815,00) diferente da base ações-planejamento (R$ 2.244.815,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>A uo 3051, programa 16, ação 4018, função 19, subfunção 571 está com valor do ano 0, base qdd-plurianual (R$ 31.454.979,00) diferente da base ações-planejamento (R$ 31.564.979,00). Diferença de R$ -110000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>A uo 4251, programa 71, ação 2074, função 8, subfunção 244 está com valor do ano 0, base qdd-plurianual (R$ 213.000,00) diferente da base ações-planejamento (R$ 1.213.000,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 58, ação 4121, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 2.432.886.227,00) diferente da base ações-planejamento (R$ 2.652.501.397,00). Diferença de R$ -219615170.</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 58, ação 4123, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 213.825.175,00) diferente da base ações-planejamento (R$ 267.869.644,00). Diferença de R$ -54044469.</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 60, ação 4125, função 10, subfunção 301 está com valor do ano 0, base qdd-plurianual (R$ 449.100.000,00) diferente da base ações-planejamento (R$ 1.038.756.948,00). Diferença de R$ -589656948.</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 60, ação 4127, função 10, subfunção 301 está com valor do ano 0, base qdd-plurianual (R$ 135.732.206,00) diferente da base ações-planejamento (R$ 332.118.192,00). Diferença de R$ -196385986.</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 61, ação 4129, função 10, subfunção 242 está com valor do ano 0, base qdd-plurianual (R$ 218.709.539,00) diferente da base ações-planejamento (R$ 221.549.539,00). Diferença de R$ -2840000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 61, ação 4130, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 122.691.215,00) diferente da base ações-planejamento (R$ 126.051.462,00). Diferença de R$ -3360247.</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 61, ação 4131, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 364.234.946,00) diferente da base ações-planejamento (R$ 367.234.946,00). Diferença de R$ -3e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 62, ação 4135, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 1.255.000,00) diferente da base ações-planejamento (R$ 25.261.085,00). Diferença de R$ -24006085.</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>A uo 4291, programa 705, ação 2500, função 10, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 261.990.084,00) diferente da base ações-planejamento (R$ 303.872.066,00). Diferença de R$ -41881982.</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>A uo 4491, programa 102, ação 4360, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 31.999.000,00) diferente da base ações-planejamento (R$ 32.999.000,00). Diferença de R$ -1e+06.</t>
         </is>
       </c>
     </row>
@@ -1637,7 +4280,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1658,141 +4301,171 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>check_count_acoes_is_deleted</t>
+          <t>check_count_programas</t>
         </is>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>check_fechamento_fonte_orcam_fiscal</t>
+          <t>check_count_acoes</t>
         </is>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_exists</t>
+          <t>check_count_acoes_is_deleted</t>
         </is>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
         </is>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>check_indicadores_justificativa_indice_referencia_em_apuracao</t>
+          <t>check_indicadores_consistency_indice_de_referencia_exists</t>
         </is>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>check_indicadores_indice_referencia_data_futura</t>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
         </is>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>check_indicadores_previsoes_zeradas</t>
+          <t>check_indicadores_indice_referencia_data_futura</t>
         </is>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>check_intra_detalhamento</t>
+          <t>check_indicadores_previsoes_zeradas</t>
         </is>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>check_limite_ano0</t>
+          <t>check_intra_detalhamento</t>
         </is>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>check_objetivos_estrategicos_exists</t>
+          <t>check_limite_ano0</t>
         </is>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>check_ods_exists</t>
+          <t>check_objetivos_estrategicos_exists</t>
         </is>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>check_setor_governo</t>
+          <t>check_ods_exists</t>
         </is>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>check_valores_qdd_fiscal</t>
+          <t>check_setor_governo</t>
         </is>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>check_valores_qdd_plurianual</t>
+          <t>check_valores_sigplan_localizadores</t>
         </is>
       </c>
       <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_programas</t>
+        </is>
+      </c>
+      <c r="B16">
         <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data package at: 2026-01-20T23:34:18Z
</commit_message>
<xml_diff>
--- a/data/checks-planejamento.xlsx
+++ b/data/checks-planejamento.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B326"/>
+  <dimension ref="A1:B548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4268,6 +4268,2673 @@
         </is>
       </c>
       <c r="B326" t="inlineStr">
+        <is>
+          <t>A uo 4491, programa 102, ação 4360, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 31.999.000,00) diferente da base ações-planejamento (R$ 32.999.000,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>check_count_programas</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>O programa 127 não consta na base localizadores, em detrimento das bases programas e ações-planejamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>check_count_acoes</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>A ação 2106, uo 1251, consta na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>check_count_acoes</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>A ação 4418, uo 1261, consta na base ações-planejamento (desc.: ESCOLA SEGURA ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>check_count_acoes</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>A ação 2103, uo 1401, consta na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>check_count_acoes</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>A ação 2104, uo 1401, consta na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>check_count_acoes</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>A ação 4411, uo 2311, consta na base ações-planejamento (desc.: GESTÃO DO ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>A ação 2108, uo 1251, consta como deletada na base ações-planejamento (desc.: FORTALECIMENTO DO ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>A ação 2500, uo 1261, consta como deletada na base ações-planejamento (desc.: ASSESSORAMENTO E ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>A ação 4161, uo 1321, consta como deletada na base ações-planejamento (desc.: VIGILÂNCIA DA ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>A ação 4177, uo 1321, consta como deletada na base ações-planejamento (desc.: VIGILÂNCIA DA ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>A ação 1026, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>A ação 1027, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>A ação 1029, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>A ação 1031, uo 2421, consta como deletada na base ações-planejamento (desc.: PROMOÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>A ação 2417, uo 2421, consta como deletada na base ações-planejamento (desc.: REMUNERAÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>A ação 2417, uo 2471, consta como deletada na base ações-planejamento (desc.: REMUNERAÇÃO DE ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>A ação 2500, uo 2471, consta como deletada na base ações-planejamento (desc.: ASSESSORAMENTO E ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>check_count_acoes_is_deleted</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>A ação 1034, uo 3041, consta como deletada na base ações-planejamento (desc.: MELHORAMENTO GENÉTICO ...) em inconsistência com a base localizadores (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 10 está com os valores totais de receita e despesa diferentes nas bases. R$ 84.363.501.073,00 na base orçamento fiscal da receita, e 89.479.183.305,00 na qdd fiscal. A diferença é de R$ -5115682232.</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 12 está com os valores totais de receita e despesa diferentes nas bases. R$ 444,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 444.</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 20 está com os valores totais de receita e despesa diferentes nas bases. R$ 0,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ NA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 31 está com os valores totais de receita e despesa diferentes nas bases. R$ 77.971.087,00 na base orçamento fiscal da receita, e 57.420.824,00 na qdd fiscal. A diferença é de R$ 20550263.</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 40 está com os valores totais de receita e despesa diferentes nas bases. R$ 392.059,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 392059.</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 46 está com os valores totais de receita e despesa diferentes nas bases. R$ 2.072,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 2072.</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 47 está com os valores totais de receita e despesa diferentes nas bases. R$ 28.687.328,00 na base orçamento fiscal da receita, e 14.640.082,00 na qdd fiscal. A diferença é de R$ 14047246.</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 52 está com os valores totais de receita e despesa diferentes nas bases. R$ 52.340.332,00 na base orçamento fiscal da receita, e 24.743.178,00 na qdd fiscal. A diferença é de R$ 27597154.</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 53 está com os valores totais de receita e despesa diferentes nas bases. R$ 1.600,00 na base orçamento fiscal da receita, e  NA na qdd fiscal. A diferença é de R$ 1600.</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 54 está com os valores totais de receita e despesa diferentes nas bases. R$ 6.682.512,00 na base orçamento fiscal da receita, e 4.104.010,00 na qdd fiscal. A diferença é de R$ 2578502.</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 59 está com os valores totais de receita e despesa diferentes nas bases. R$ 383.447.752,00 na base orçamento fiscal da receita, e 342.620.315,00 na qdd fiscal. A diferença é de R$ 40827437.</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 60 está com os valores totais de receita e despesa diferentes nas bases. R$ 4.528.328.118,00 na base orçamento fiscal da receita, e 3.795.212.434,00 na qdd fiscal. A diferença é de R$ 733115684.</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 61 está com os valores totais de receita e despesa diferentes nas bases. R$ 433.782.405,00 na base orçamento fiscal da receita, e 406.710.026,00 na qdd fiscal. A diferença é de R$ 27072379.</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 72 está com os valores totais de receita e despesa diferentes nas bases. R$ 456.921.538,00 na base orçamento fiscal da receita, e 350.859.025,00 na qdd fiscal. A diferença é de R$ 106062513.</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 79 está com os valores totais de receita e despesa diferentes nas bases. R$ 7.765.658,00 na base orçamento fiscal da receita, e 4.000.000,00 na qdd fiscal. A diferença é de R$ 3765658.</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 83 está com os valores totais de receita e despesa diferentes nas bases. R$ 205.514.880,00 na base orçamento fiscal da receita, e 175.581.839,00 na qdd fiscal. A diferença é de R$ 29933041.</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 91 está com os valores totais de receita e despesa diferentes nas bases. R$ 133.921.299,00 na base orçamento fiscal da receita, e 69.063.939,00 na qdd fiscal. A diferença é de R$ 64857360.</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>check_fechamento_fonte_orcam_fiscal</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>A Fonte de Recurso 94 está com os valores totais de receita e despesa diferentes nas bases. R$ 10.715.576,00 na base orçamento fiscal da receita, e 6.760.698,00 na qdd fiscal. A diferença é de R$ 3954878.</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_exists</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>O programa 2 contém indicador (PERCENTUAL DE INSTITUCIONALIZAÇÃO...) que, apesar de ter índice de referência de 100, está sem meta para o ano 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>O programa 3 contém indicador (ÍNDICE DE EFETIVIDADE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>O programa 11 contém indicador (TAXA DE MATERIAIS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>O programa 18 contém indicador (NUMERO DE MATÉRIAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>O programa 27 contém indicador (INCREMENTO DE ABRANGÊNCIA...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>O programa 27 contém indicador (ABRANGÊNCIA DOS PROGRAMAS,...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>O programa 27 contém indicador (EXECUÇÃO DAS METAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>O programa 81 contém indicador (EVOLUÇÃO DA QUALIDADE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>O programa 91 contém indicador (DISCENTES FORMADOS E...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>O programa 91 contém indicador (GRAU DE SATISFAÇÃO...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>O programa 91 contém indicador (ARTIGOS ACADÊMICOS ACEITOS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>O programa 99 contém indicador (ÍNDICE ACUMULADO DE...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>O programa 172 contém indicador (PERCENTUAL DE EXECUÇÃO...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>O programa 172 contém indicador (PERCENTUAL DE OBRAS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>O programa 746 contém indicador (QUANTIDADE DE INDÍCIOS...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>check_indicadores_consistency_indice_de_referencia_missing</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>O programa 746 contém indicador (ÍNDICE DE IRREGULARIDADES...) que, apesar não de ter índice de referência, está com meta para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>check_indicadores_indice_referencia_data_futura</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>O programa 64 contém indicador (NÚMERO DE MUNICÍPIOS...) cujo índice de referência, apesar de não estar em apuração, apresenta data de apuração futura: 2025-12-31.</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>O programa 92 contém indicador (TAXA DE EXPANSÃO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>O programa 94 contém indicador (TAXA DE CRESCIMENTO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>O programa 165 contém indicador (IDEB ANOS INICIAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>O programa 165 contém indicador (IDEB ENSINO MÉDIO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>O programa 165 contém indicador (IDEB ANOS FINAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>O programa 167 contém indicador (IDEB ANOS INICIAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>O programa 167 contém indicador (IDEB ENSINO MÉDIO...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>check_indicadores_previsoes_zeradas</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>O programa 167 contém indicador (IDEB ANOS FINAIS...) cuja previsão, apesar de não estar em apuração, está com valor zerado para o ano 3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>A uo 1401 está com valor recebido de recursos intraorçamentários (R$ 960.756,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>A uo 1451 está com valor recebido de recursos intraorçamentários (R$ 224.346.201,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>A uo 1541 está com valor recebido de recursos intraorçamentários (R$ 31.538.282,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>A uo 2011 está com valor recebido de recursos intraorçamentários (R$ 647.702.182,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>A uo 2121 está com valor recebido de recursos intraorçamentários (R$ 2.260.804.301,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>A uo 2251 está com valor recebido de recursos intraorçamentários (R$ 18.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>A uo 2261 está com valor recebido de recursos intraorçamentários (R$ 652.857.538,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>A uo 2271 está com valor recebido de recursos intraorçamentários (R$ 2.397.229.409,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>A uo 2321 está com valor recebido de recursos intraorçamentários (R$ 487.249.378,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>A uo 2361 está com valor recebido de recursos intraorçamentários (R$ 15.037.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>A uo 3051 está com valor recebido de recursos intraorçamentários (R$ 660.084,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>A uo 4031 está com valor recebido de recursos intraorçamentários (R$ 87.655.976,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>A uo 4631 está com valor recebido de recursos intraorçamentários (R$ 1.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>A uo 4661 está com valor recebido de recursos intraorçamentários (R$ 470.000,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>A uo 4711 está com valor recebido de recursos intraorçamentários (R$ 7.218.864.598,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>check_intra_detalhamento</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>A uo 9901 está com valor recebido de recursos intraorçamentários (R$ 580.295.911,00) diferente do valor detalhado (R$ 0,00) na base intra-detalhamento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>A uo 1231 está com uma diferença de R$ (15.387,00) entre o valor de limite no ano 0 (R$ 12.495.112,00) e a soma do valor utilizado no ano (R$ 12.510.499,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 12.510.499,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>A uo 1301 está com uma diferença de R$ (1.000,00) entre o valor de limite no ano 0 (R$ 29.425.835,00) e a soma do valor utilizado no ano (R$ 29.426.835,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 29.426.835,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>A uo 1451 está com uma diferença de R$ (150.714.182,00) entre o valor de limite no ano 0 (R$ 353.708.669,00) e a soma do valor utilizado no ano (R$ 504.422.851,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 504.422.851,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>A uo 1451 está com uma diferença de R$ (1.778.147,00) entre o valor de limite no ano 0 (R$ 41.116.142,00) e a soma do valor utilizado no ano (R$ 42.894.289,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 42.894.289,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>A uo 2171 está com uma diferença de R$ (2.000,00) entre o valor de limite no ano 0 (R$ 2.641.831,00) e a soma do valor utilizado no ano (R$ 2.643.831,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 2.643.831,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>A uo 2171 está com uma diferença de R$ (45.346,00) entre o valor de limite no ano 0 (R$ 1.145.946,00) e a soma do valor utilizado no ano (R$ 1.191.292,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 1.191.292,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>A uo 2371 está com uma diferença de R$ (26.250,00) entre o valor de limite no ano 0 (R$ 87.500,00) e a soma do valor utilizado no ano (R$ 113.750,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 113.750,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>check_limite_ano0</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>A uo 4291 está com uma diferença de R$ 1.034.956.298,00 entre o valor de limite no ano 0 (R$ 1.389.694.094,00) e a soma do valor utilizado no ano (R$ 354.737.796,00) com o valor transferido no ano (R$ 0,00), que totalizam R$ 354.737.796,00.</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>O programa 98 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>O programa 704 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>O programa 706 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>O programa 726 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>O programa 729 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>O programa 734 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>O programa 738 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>O programa 746 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>O programa 760 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>O programa 764 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>O programa 765 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>O programa 766 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>check_objetivos_estrategicos_exists</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>O programa 767 está sem objetivo estratégico válido na base programas-planejamento (3-Não há objetivo estratégico vinculado.). Cada programa precisa ter pelo menos um objetivo estratégico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>check_ods_exists</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>O programa 8 está sem objetivo de desenvolvimento estratégico definido.</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>check_ods_exists</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>O programa 126 está sem objetivo de desenvolvimento estratégico definido.</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>check_ods_exists</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>O programa 138 está sem objetivo de desenvolvimento estratégico definido.</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>check_ods_exists</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>O programa 142 está sem objetivo de desenvolvimento estratégico definido.</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>check_setor_governo</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>A uo 1321 está com setor divergente na base ações-planejamento (SAÚDE) em relação à tabela auxiliar setor-governo da loa (NA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>check_setor_governo</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>A uo 1917 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (FAZENDA).</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>check_setor_governo</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>A uo 4171 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (AGRICULTURA, PECUÁRIA E ABASTECIMENTO).</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>check_setor_governo</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>A uo 4531 está com setor divergente na base ações-planejamento (NA) em relação à tabela auxiliar setor-governo da loa (DESENVOLVIMENTO ECONÔMICO).</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 127, ação 2106, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 127, ação 4418, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4124, função 18, subfunção 541, área temática 11AT11 está com valor de meta orçamentária do ano 0, base localizadores (R$ 4.000.000,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ -4e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 127, ação 2104, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 165, ação 2103, função 12, subfunção 368, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>A uo 1441, programa 726, ação 4193, função 3, subfunção 92, área temática 15AT15 está com valor de meta orçamentária do ano 0, base localizadores (R$ 850.658.836,00) diferente da base ações-planejamento (R$ 4.361.285,00). Diferença de R$ -846297551.</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 146, ação 4442, função 12, subfunção 243, área temática 07AT07 está com valor de meta orçamentária do ano 0, base localizadores (R$ 136.139.820,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ -136139820.</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>A uo 1991, programa 999, ação 9999, função 99, subfunção 999, área temática 08AT08 está com valor de meta orçamentária do ano 0, base localizadores (R$ 1.207.332.593,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ -1207332593.</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_localizadores</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4411, função 10, subfunção 302, área temática 03AT03 está com valor de meta orçamentária do ano 0, base localizadores (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>check_valores_sigplan_programas</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>A uo 2311, 
+programa 7, 
+área temática 03AT03 está com valor 
+de meta orçamentária do ano 0, base programas (R$ 187.558.168,00) diferente da base ações-planejamento (R$  NA). Diferença de R$ 187558168.</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 127, ação 2106, função 12, subfunção 368 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 127, ação 4418, função 12, subfunção 368 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4124, função 18, subfunção 541 está com valor na base qdd-fiscal (R$ 4.000.000,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 4e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 127, ação 2104, função 12, subfunção 368 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 165, ação 2103, função 12, subfunção 368 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>A uo 1441, programa 726, ação 4193, função 3, subfunção 92 está com valor na base qdd-fiscal (R$ 850.658.836,00) diferente da base ações-planejamento (R$ 4.361.285,00). Diferença de R$ 846297551.</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 146, ação 4442, função 12, subfunção 243 está com valor na base qdd-fiscal (R$ 136.139.820,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 136139820.</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>A uo 1991, programa 999, ação 9999, função 99, subfunção 999 está com valor na base qdd-fiscal (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_fiscal</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4411, função 10, subfunção 302 está com valor na base qdd-fiscal (R$ 1.000,00) diferente da base ações-planejamento (R$  NA). Diferença de R$ 1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 746, ação 2009, função 1, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 199.226.735,00) diferente da base ações-planejamento (R$ 202.637.401,00). Diferença de R$ -3410666.</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>A uo 1021, programa 760, ação 2145, função 1, subfunção 128 está com valor do ano 0, base qdd-plurianual (R$ 8.462.193,00) diferente da base ações-planejamento (R$ 12.662.193,00). Diferença de R$ -4200000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>A uo 1071, programa 48, ação 4155, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 131.000,00) diferente da base ações-planejamento (R$ 1.731.000,00). Diferença de R$ -1600000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>A uo 1071, programa 101, ação 1008, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 14.800.970,00) diferente da base ações-planejamento (R$ 17.060.970,00). Diferença de R$ -2260000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>A uo 1221, programa 125, ação 1082, função 4, subfunção 127 está com valor do ano 0, base qdd-plurianual (R$ 47.501.208,00) diferente da base ações-planejamento (R$ 48.281.208,00). Diferença de R$ -780000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>A uo 1221, programa 132, ação 4474, função 23, subfunção 691 está com valor do ano 0, base qdd-plurianual (R$ 617.333,00) diferente da base ações-planejamento (R$ 1.117.333,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 108, ação 4358, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 9.441.948,00) diferente da base ações-planejamento (R$ 11.326.448,00). Diferença de R$ -1884500.</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 110, ação 4363, função 21, subfunção 605 está com valor do ano 0, base qdd-plurianual (R$ 8.311.853,00) diferente da base ações-planejamento (R$ 9.061.853,00). Diferença de R$ -750000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 111, ação 4383, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 13.387.942,00) diferente da base ações-planejamento (R$ 13.537.942,00). Diferença de R$ -150000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 111, ação 4420, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 30.000.000,00) diferente da base ações-planejamento (R$ 53.592.878,00). Diferença de R$ -23592878.</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 112, ação 4403, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 5.720.025,00) diferente da base ações-planejamento (R$ 5.810.235,00). Diferença de R$ -90210.</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 114, ação 4398, função 20, subfunção 607 está com valor do ano 0, base qdd-plurianual (R$ 11.866.753,00) diferente da base ações-planejamento (R$ 13.841.359,00). Diferença de R$ -1974606.</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 114, ação 4419, função 20, subfunção 127 está com valor do ano 0, base qdd-plurianual (R$ 1.377.192,00) diferente da base ações-planejamento (R$ 2.377.192,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>A uo 1231, programa 705, ação 2500, função 20, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 12.430.883,00) diferente da base ações-planejamento (R$ 13.930.883,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 127, ação 2106, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4365, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 6.334.166.724,00) diferente da base ações-planejamento (R$ 6.334.866.724,00). Diferença de R$ -7e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4366, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 1.050,00) diferente da base ações-planejamento (R$ 40.343.178,00). Diferença de R$ -40342128.</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 137, ação 4373, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 3.600,00) diferente da base ações-planejamento (R$ 103.600,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>A uo 1251, programa 705, ação 2500, função 6, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 376.861.077,00) diferente da base ações-planejamento (R$ 378.361.077,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 127, ação 4418, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 167, ação 2122, função 12, subfunção 361 está com valor do ano 0, base qdd-plurianual (R$ 117.100.000,00) diferente da base ações-planejamento (R$ 118.550.000,00). Diferença de R$ -1450000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 167, ação 4511, função 12, subfunção 362 está com valor do ano 0, base qdd-plurianual (R$ 62.600.000,00) diferente da base ações-planejamento (R$ 66.600.000,00). Diferença de R$ -4e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 2126, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$ 456.147.344,00) diferente da base ações-planejamento (R$ 553.858.039,00). Diferença de R$ -97710695.</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 4519, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$ 524.704.215,00) diferente da base ações-planejamento (R$ 534.715.902,00). Diferença de R$ -10011687.</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 168, ação 4527, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$ 644.976.000,00) diferente da base ações-planejamento (R$ 650.592.317,00). Diferença de R$ -5616317.</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>A uo 1261, programa 172, ação 4545, função 12, subfunção 361 está com valor do ano 0, base qdd-plurianual (R$ 45.000.000,00) diferente da base ações-planejamento (R$ 45.324.049,00). Diferença de R$ -324049.</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 102, ação 4332, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 33.144.232,00) diferente da base ações-planejamento (R$ 49.994.232,00). Diferença de R$ -16850000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 102, ação 4343, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 170.568.000,00) diferente da base ações-planejamento (R$ 170.569.000,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 103, ação 4322, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 10.500.000,00) diferente da base ações-planejamento (R$ 10.800.000,00). Diferença de R$ -3e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>A uo 1271, programa 705, ação 2500, função 13, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 2.820.327,00) diferente da base ações-planejamento (R$ 3.320.327,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>A uo 1301, programa 99, ação 4261, função 15, subfunção 451 está com valor do ano 0, base qdd-plurianual (R$ 7.140.411,00) diferente da base ações-planejamento (R$ 10.140.411,00). Diferença de R$ -3e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>A uo 1301, programa 99, ação 4262, função 15, subfunção 451 está com valor do ano 0, base qdd-plurianual (R$ 16.016.092,00) diferente da base ações-planejamento (R$ 35.016.092,00). Diferença de R$ -1.9e+07.</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 21, ação 4028, função 17, subfunção 512 está com valor do ano 0, base qdd-plurianual (R$ 50.231.475,00) diferente da base ações-planejamento (R$ 51.439.475,00). Diferença de R$ -1208000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 21, ação 4044, função 17, subfunção 512 está com valor do ano 0, base qdd-plurianual (R$ 3.819.644,00) diferente da base ações-planejamento (R$ 4.219.644,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4045, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 807.634,00) diferente da base ações-planejamento (R$ 2.807.634,00). Diferença de R$ -2e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4046, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 557.957,00) diferente da base ações-planejamento (R$ 558.957,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4047, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 685.640,00) diferente da base ações-planejamento (R$ 34.385.640,00). Diferença de R$ -33700000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>A uo 1371, programa 27, ação 4124, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 3.200.000,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 3200000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4114, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 486.636.314,00) diferente da base ações-planejamento (R$ 494.723.314,00). Diferença de R$ -8087000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4115, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 687.674.923,00) diferente da base ações-planejamento (R$ 688.174.923,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4120, função 6, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 11.030.599,00) diferente da base ações-planejamento (R$ 14.160.599,00). Diferença de R$ -3130000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 52, ação 4138, função 18, subfunção 182 está com valor do ano 0, base qdd-plurianual (R$ 11.690.903,00) diferente da base ações-planejamento (R$ 12.690.903,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 53, ação 4094, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 960.756,00) diferente da base ações-planejamento (R$ 8.281.747,00). Diferença de R$ -7320991.</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 127, ação 2104, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>A uo 1401, programa 165, ação 2103, função 12, subfunção 368 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 0.</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>A uo 1441, programa 726, ação 4193, função 3, subfunção 92 está com valor do ano 0, base qdd-plurianual (R$ 850.658.836,00) diferente da base ações-planejamento (R$ 4.361.285,00). Diferença de R$ 846297551.</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 129, ação 4344, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 51.978.801,00) diferente da base ações-planejamento (R$ 52.679.791,00). Diferença de R$ -700990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 129, ação 4347, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 2.002.000,00) diferente da base ações-planejamento (R$ 2.003.000,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 1048, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 58.811.637,00) diferente da base ações-planejamento (R$ 63.784.579,00). Diferença de R$ -4972942.</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 4348, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 735.242.265,00) diferente da base ações-planejamento (R$ 736.174.265,00). Diferença de R$ -932000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 130, ação 4351, função 6, subfunção 421 está com valor do ano 0, base qdd-plurianual (R$ 124.967.835,00) diferente da base ações-planejamento (R$ 125.067.835,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 141, ação 4438, função 6, subfunção 422 está com valor do ano 0, base qdd-plurianual (R$ 6.775.354,00) diferente da base ações-planejamento (R$ 7.275.354,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>A uo 1451, programa 146, ação 4442, função 12, subfunção 243 está com valor do ano 0, base qdd-plurianual (R$ 136.139.820,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 136139820.</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 66, ação 4153, função 11, subfunção 334 está com valor do ano 0, base qdd-plurianual (R$ 6.876.017,00) diferente da base ações-planejamento (R$ 7.126.017,00). Diferença de R$ -250000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4167, função 27, subfunção 812 está com valor do ano 0, base qdd-plurianual (R$ 1.187.363,00) diferente da base ações-planejamento (R$ 1.687.363,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4170, função 27, subfunção 812 está com valor do ano 0, base qdd-plurianual (R$ 1.374.510,00) diferente da base ações-planejamento (R$ 11.159.340,00). Diferença de R$ -9784830.</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 69, ação 4514, função 27, subfunção 812 está com valor do ano 0, base qdd-plurianual (R$ 3.378.169,00) diferente da base ações-planejamento (R$ 3.628.169,00). Diferença de R$ -250000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 70, ação 4174, função 14, subfunção 422 está com valor do ano 0, base qdd-plurianual (R$ 1.000,00) diferente da base ações-planejamento (R$ 2.001.990,00). Diferença de R$ -2000990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 74, ação 4196, função 14, subfunção 306 está com valor do ano 0, base qdd-plurianual (R$ 1.242.678,00) diferente da base ações-planejamento (R$ 1.642.678,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 86, ação 4415, função 14, subfunção 422 está com valor do ano 0, base qdd-plurianual (R$ 2.622.178,00) diferente da base ações-planejamento (R$ 2.722.178,00). Diferença de R$ -1e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>A uo 1481, programa 148, ação 2079, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 5.634.602,00) diferente da base ações-planejamento (R$ 16.425.592,00). Diferença de R$ -10790990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>A uo 1491, programa 119, ação 2045, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 3.189.678,00) diferente da base ações-planejamento (R$ 98.946.739,00). Diferença de R$ -95757061.</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>A uo 1491, programa 119, ação 2048, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 1.000,00) diferente da base ações-planejamento (R$ 861.067.452,00). Diferença de R$ -861066452.</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>A uo 1501, programa 156, ação 4465, função 4, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 95.680.170,00) diferente da base ações-planejamento (R$ 96.243.170,00). Diferença de R$ -563000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 1006, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 316,00) diferente da base ações-planejamento (R$ 500.316,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 1007, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 1.000,00) diferente da base ações-planejamento (R$ 21.138.490,00). Diferença de R$ -21137490.</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 4060, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 158.599.650,00) diferente da base ações-planejamento (R$ 161.249.650,00). Diferença de R$ -2650000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>A uo 1511, programa 32, ação 4061, função 6, subfunção 181 está com valor do ano 0, base qdd-plurianual (R$ 14.695.363,00) diferente da base ações-planejamento (R$ 14.845.363,00). Diferença de R$ -150000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>A uo 1991, programa 999, ação 9999, função 99, subfunção 999 está com valor do ano 1, base qdd-plurianual (R$ 1.244.759.904,00) diferente da base ações-planejamento (R$ 0,00). Diferença de R$ 1244759904.</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>A uo 2071, programa 22, ação 4513, função 19, subfunção 571 está com valor do ano 0, base qdd-plurianual (R$ 182.314.608,00) diferente da base ações-planejamento (R$ 182.514.607,00). Diferença de R$ -199999.</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>A uo 2101, programa 31, ação 4056, função 18, subfunção 543 está com valor do ano 0, base qdd-plurianual (R$ 26.736.707,00) diferente da base ações-planejamento (R$ 27.136.707,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>A uo 2101, programa 31, ação 4059, função 18, subfunção 541 está com valor do ano 0, base qdd-plurianual (R$ 55.956.871,00) diferente da base ações-planejamento (R$ 57.356.871,00). Diferença de R$ -1400000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>A uo 2201, programa 106, ação 4276, função 13, subfunção 391 está com valor do ano 0, base qdd-plurianual (R$ 63.050,00) diferente da base ações-planejamento (R$ 598.050,00). Diferença de R$ -535000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>A uo 2201, programa 106, ação 4278, função 13, subfunção 391 está com valor do ano 0, base qdd-plurianual (R$ 848.458,00) diferente da base ações-planejamento (R$ 1.348.458,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>A uo 2271, programa 19, ação 4031, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 403.048.770,00) diferente da base ações-planejamento (R$ 403.408.770,00). Diferença de R$ -360000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>A uo 2271, programa 19, ação 4036, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$ 203.935.708,00) diferente da base ações-planejamento (R$ 204.475.708,00). Diferença de R$ -540000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4268, função 26, subfunção 782 está com valor do ano 0, base qdd-plurianual (R$ 88.091.501,00) diferente da base ações-planejamento (R$ 88.092.501,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4275, função 26, subfunção 782 está com valor do ano 0, base qdd-plurianual (R$ 363.158.594,00) diferente da base ações-planejamento (R$ 363.159.594,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>A uo 2301, programa 81, ação 4293, função 26, subfunção 782 está com valor do ano 0, base qdd-plurianual (R$ 651.192.418,00) diferente da base ações-planejamento (R$ 651.193.418,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4002, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 3.958.056,00) diferente da base ações-planejamento (R$ 5.458.056,00). Diferença de R$ -1500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4005, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 4.525.088,00) diferente da base ações-planejamento (R$ 9.525.088,00). Diferença de R$ -5e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 7, ação 4411, função 10, subfunção 302 está com valor do ano 0, base qdd-plurianual (R$  NA) diferente da base ações-planejamento (R$  NA). Diferença de R$ NA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>A uo 2311, programa 705, ação 2500, função 12, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 10.931.901,00) diferente da base ações-planejamento (R$ 11.431.901,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4086, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 115.679.715,00) diferente da base ações-planejamento (R$ 117.379.715,00). Diferença de R$ -1700000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4087, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 5.959.778,00) diferente da base ações-planejamento (R$ 5.960.778,00). Diferença de R$ -1000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4089, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 6.377.753,00) diferente da base ações-planejamento (R$ 10.977.753,00). Diferença de R$ -4600000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>A uo 2351, programa 26, ação 4090, função 12, subfunção 364 está com valor do ano 0, base qdd-plurianual (R$ 24.069.722,00) diferente da base ações-planejamento (R$ 24.909.722,00). Diferença de R$ -840000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 101, ação 1016, função 8, subfunção 544 está com valor do ano 0, base qdd-plurianual (R$ 4.842.287,00) diferente da base ações-planejamento (R$ 5.957.287,00). Diferença de R$ -1115000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 101, ação 1032, função 8, subfunção 544 está com valor do ano 0, base qdd-plurianual (R$ 3.206.136,00) diferente da base ações-planejamento (R$ 9.447.126,00). Diferença de R$ -6240990.</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 124, ação 4325, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 648.218,00) diferente da base ações-planejamento (R$ 1.048.218,00). Diferença de R$ -4e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>A uo 2421, programa 124, ação 4516, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 411.620,00) diferente da base ações-planejamento (R$ 3.911.620,00). Diferença de R$ -3500000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 90, ação 4235, função 20, subfunção 606 está com valor do ano 0, base qdd-plurianual (R$ 92.806.224,00) diferente da base ações-planejamento (R$ 95.106.224,00). Diferença de R$ -2300000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 97, ação 4236, função 20, subfunção 608 está com valor do ano 0, base qdd-plurianual (R$ 58.536.458,00) diferente da base ações-planejamento (R$ 78.162.208,00). Diferença de R$ -19625750.</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>A uo 3041, programa 705, ação 2500, função 20, subfunção 122 está com valor do ano 0, base qdd-plurianual (R$ 1.744.815,00) diferente da base ações-planejamento (R$ 2.244.815,00). Diferença de R$ -5e+05.</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>A uo 3051, programa 16, ação 4018, função 19, subfunção 571 está com valor do ano 0, base qdd-plurianual (R$ 31.454.979,00) diferente da base ações-planejamento (R$ 31.564.979,00). Diferença de R$ -110000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>A uo 4251, programa 71, ação 2074, função 8, subfunção 244 está com valor do ano 0, base qdd-plurianual (R$ 213.000,00) diferente da base ações-planejamento (R$ 1.213.000,00). Diferença de R$ -1e+06.</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>check_valores_qdd_plurianual</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
         <is>
           <t>A uo 4491, programa 102, ação 4360, função 13, subfunção 392 está com valor do ano 0, base qdd-plurianual (R$ 31.999.000,00) diferente da base ações-planejamento (R$ 32.999.000,00). Diferença de R$ -1e+06.</t>
         </is>
@@ -4305,7 +6972,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -4315,7 +6982,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -4325,7 +6992,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -4335,7 +7002,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
@@ -4345,7 +7012,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -4355,7 +7022,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
@@ -4365,7 +7032,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -4375,7 +7042,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -4385,7 +7052,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -4395,7 +7062,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -4405,7 +7072,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
@@ -4415,7 +7082,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -4425,7 +7092,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -4435,7 +7102,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -4445,7 +7112,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -4455,7 +7122,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18">
@@ -4465,7 +7132,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>107</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>